<commit_message>
add "no" for empty values
</commit_message>
<xml_diff>
--- a/titlePilotStudy/data/ITL.xlsx
+++ b/titlePilotStudy/data/ITL.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roxana\Desktop\CONFERINTE toamna 2019\malaga 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HU-BOX\Seafile\COST\dataTitleStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="231">
   <si>
     <t>ITBI0087</t>
   </si>
@@ -1139,8 +1139,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1156,7 +1156,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1420,15 +1420,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O1" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="AB37" sqref="AB37"/>
+      <selection pane="bottomLeft" activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +1546,9 @@
       <c r="K2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M2" s="5" t="s">
         <v>140</v>
       </c>
@@ -1556,8 +1558,12 @@
       <c r="O2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="P2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R2" s="5" t="s">
         <v>140</v>
       </c>
@@ -1588,9 +1594,11 @@
       <c r="AA2" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB2" s="6"/>
-    </row>
-    <row r="3" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="AB2" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1622,7 +1630,9 @@
       <c r="K3" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M3" s="5" t="s">
         <v>140</v>
       </c>
@@ -1632,8 +1642,12 @@
       <c r="O3" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="P3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R3" s="5" t="s">
         <v>140</v>
       </c>
@@ -1664,9 +1678,11 @@
       <c r="AA3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB3" s="6"/>
-    </row>
-    <row r="4" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="AB3" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1698,7 +1714,9 @@
       <c r="K4" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L4" s="5"/>
+      <c r="L4" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M4" s="5" t="s">
         <v>140</v>
       </c>
@@ -1708,7 +1726,9 @@
       <c r="O4" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P4" s="5"/>
+      <c r="P4" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q4" s="5" t="s">
         <v>147</v>
       </c>
@@ -1746,7 +1766,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1790,8 +1810,12 @@
       <c r="O5" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+      <c r="P5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R5" s="5" t="s">
         <v>140</v>
       </c>
@@ -1804,7 +1828,9 @@
       <c r="U5" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V5" s="5"/>
+      <c r="V5" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W5" s="5" t="s">
         <v>140</v>
       </c>
@@ -1820,9 +1846,11 @@
       <c r="AA5" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB5" s="6"/>
-    </row>
-    <row r="6" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="AB5" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1854,7 +1882,9 @@
       <c r="K6" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M6" s="5" t="s">
         <v>140</v>
       </c>
@@ -1864,8 +1894,12 @@
       <c r="O6" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="P6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R6" s="5" t="s">
         <v>140</v>
       </c>
@@ -1896,9 +1930,11 @@
       <c r="AA6" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB6" s="6"/>
-    </row>
-    <row r="7" spans="1:28" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="AB6" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1930,7 +1966,9 @@
       <c r="K7" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L7" s="5"/>
+      <c r="L7" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M7" s="5" t="s">
         <v>140</v>
       </c>
@@ -1940,7 +1978,9 @@
       <c r="O7" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P7" s="5"/>
+      <c r="P7" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q7" s="5" t="s">
         <v>148</v>
       </c>
@@ -1976,7 +2016,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -2008,7 +2048,9 @@
       <c r="K8" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M8" s="5" t="s">
         <v>140</v>
       </c>
@@ -2018,8 +2060,12 @@
       <c r="O8" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
+      <c r="P8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R8" s="5" t="s">
         <v>140</v>
       </c>
@@ -2050,9 +2096,11 @@
       <c r="AA8" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB8" s="6"/>
-    </row>
-    <row r="9" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="AB8" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -2084,7 +2132,9 @@
       <c r="K9" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M9" s="5" t="s">
         <v>140</v>
       </c>
@@ -2094,8 +2144,12 @@
       <c r="O9" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
+      <c r="P9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R9" s="5" t="s">
         <v>140</v>
       </c>
@@ -2126,9 +2180,11 @@
       <c r="AA9" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB9" s="6"/>
-    </row>
-    <row r="10" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="AB9" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -2160,7 +2216,9 @@
       <c r="K10" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M10" s="5" t="s">
         <v>140</v>
       </c>
@@ -2170,8 +2228,12 @@
       <c r="O10" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
+      <c r="P10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R10" s="5" t="s">
         <v>140</v>
       </c>
@@ -2202,9 +2264,11 @@
       <c r="AA10" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB10" s="6"/>
-    </row>
-    <row r="11" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="AB10" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -2236,7 +2300,9 @@
       <c r="K11" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M11" s="5" t="s">
         <v>140</v>
       </c>
@@ -2246,7 +2312,9 @@
       <c r="O11" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P11" s="5"/>
+      <c r="P11" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q11" s="5" t="s">
         <v>160</v>
       </c>
@@ -2262,7 +2330,9 @@
       <c r="U11" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V11" s="5"/>
+      <c r="V11" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W11" s="5" t="s">
         <v>140</v>
       </c>
@@ -2282,7 +2352,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -2314,7 +2384,9 @@
       <c r="K12" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M12" s="5" t="s">
         <v>140</v>
       </c>
@@ -2324,7 +2396,9 @@
       <c r="O12" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P12" s="5"/>
+      <c r="P12" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q12" s="5" t="s">
         <v>161</v>
       </c>
@@ -2340,7 +2414,9 @@
       <c r="U12" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V12" s="5"/>
+      <c r="V12" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W12" s="5" t="s">
         <v>140</v>
       </c>
@@ -2360,7 +2436,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -2392,7 +2468,9 @@
       <c r="K13" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M13" s="5" t="s">
         <v>140</v>
       </c>
@@ -2402,7 +2480,9 @@
       <c r="O13" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P13" s="5"/>
+      <c r="P13" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q13" s="5" t="s">
         <v>162</v>
       </c>
@@ -2440,7 +2520,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -2472,7 +2552,9 @@
       <c r="K14" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L14" s="5"/>
+      <c r="L14" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M14" s="5" t="s">
         <v>140</v>
       </c>
@@ -2482,8 +2564,12 @@
       <c r="O14" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="P14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R14" s="5" t="s">
         <v>140</v>
       </c>
@@ -2518,7 +2604,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
@@ -2550,7 +2636,9 @@
       <c r="K15" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M15" s="5" t="s">
         <v>140</v>
       </c>
@@ -2560,7 +2648,9 @@
       <c r="O15" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P15" s="5"/>
+      <c r="P15" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q15" s="5" t="s">
         <v>175</v>
       </c>
@@ -2576,7 +2666,9 @@
       <c r="U15" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V15" s="5"/>
+      <c r="V15" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W15" s="5" t="s">
         <v>140</v>
       </c>
@@ -2592,9 +2684,11 @@
       <c r="AA15" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB15" s="6"/>
-    </row>
-    <row r="16" spans="1:28" ht="87" x14ac:dyDescent="0.35">
+      <c r="AB15" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -2626,7 +2720,9 @@
       <c r="K16" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M16" s="5" t="s">
         <v>140</v>
       </c>
@@ -2654,7 +2750,9 @@
       <c r="U16" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V16" s="5"/>
+      <c r="V16" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W16" s="5" t="s">
         <v>140</v>
       </c>
@@ -2674,7 +2772,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>55</v>
       </c>
@@ -2706,7 +2804,9 @@
       <c r="K17" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L17" s="5"/>
+      <c r="L17" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M17" s="5" t="s">
         <v>140</v>
       </c>
@@ -2716,8 +2816,12 @@
       <c r="O17" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
+      <c r="P17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R17" s="5" t="s">
         <v>140</v>
       </c>
@@ -2752,7 +2856,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="348" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
@@ -2784,7 +2888,9 @@
       <c r="K18" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M18" s="5" t="s">
         <v>140</v>
       </c>
@@ -2794,7 +2900,9 @@
       <c r="O18" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P18" s="5"/>
+      <c r="P18" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q18" s="5" t="s">
         <v>179</v>
       </c>
@@ -2832,7 +2940,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -2864,7 +2972,9 @@
       <c r="K19" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M19" s="5" t="s">
         <v>140</v>
       </c>
@@ -2874,7 +2984,9 @@
       <c r="O19" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P19" s="5"/>
+      <c r="P19" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q19" s="5" t="s">
         <v>184</v>
       </c>
@@ -2912,7 +3024,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -2944,7 +3056,9 @@
       <c r="K20" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L20" s="5"/>
+      <c r="L20" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M20" s="5" t="s">
         <v>140</v>
       </c>
@@ -2954,7 +3068,9 @@
       <c r="O20" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P20" s="5"/>
+      <c r="P20" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q20" s="5" t="s">
         <v>187</v>
       </c>
@@ -2970,7 +3086,9 @@
       <c r="U20" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V20" s="5"/>
+      <c r="V20" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W20" s="5" t="s">
         <v>140</v>
       </c>
@@ -2990,7 +3108,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>65</v>
       </c>
@@ -3034,7 +3152,9 @@
       <c r="O21" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P21" s="5"/>
+      <c r="P21" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q21" s="5" t="s">
         <v>189</v>
       </c>
@@ -3072,7 +3192,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
@@ -3116,7 +3236,9 @@
       <c r="O22" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P22" s="5"/>
+      <c r="P22" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q22" s="5" t="s">
         <v>193</v>
       </c>
@@ -3132,7 +3254,9 @@
       <c r="U22" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V22" s="5"/>
+      <c r="V22" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W22" s="5" t="s">
         <v>140</v>
       </c>
@@ -3148,9 +3272,11 @@
       <c r="AA22" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB22" s="6"/>
-    </row>
-    <row r="23" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="AB22" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>72</v>
       </c>
@@ -3182,7 +3308,9 @@
       <c r="K23" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L23" s="5"/>
+      <c r="L23" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M23" s="5" t="s">
         <v>140</v>
       </c>
@@ -3210,7 +3338,9 @@
       <c r="U23" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V23" s="5"/>
+      <c r="V23" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W23" s="5" t="s">
         <v>140</v>
       </c>
@@ -3230,7 +3360,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>75</v>
       </c>
@@ -3262,7 +3392,9 @@
       <c r="K24" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L24" s="5"/>
+      <c r="L24" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M24" s="5" t="s">
         <v>140</v>
       </c>
@@ -3290,7 +3422,9 @@
       <c r="U24" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V24" s="5"/>
+      <c r="V24" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W24" s="5" t="s">
         <v>140</v>
       </c>
@@ -3310,7 +3444,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>78</v>
       </c>
@@ -3342,7 +3476,9 @@
       <c r="K25" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L25" s="5"/>
+      <c r="L25" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M25" s="5" t="s">
         <v>140</v>
       </c>
@@ -3352,8 +3488,12 @@
       <c r="O25" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
+      <c r="P25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R25" s="5" t="s">
         <v>140</v>
       </c>
@@ -3384,9 +3524,11 @@
       <c r="AA25" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB25" s="6"/>
-    </row>
-    <row r="26" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="AB25" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>83</v>
       </c>
@@ -3430,8 +3572,12 @@
       <c r="O26" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
+      <c r="P26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R26" s="5" t="s">
         <v>140</v>
       </c>
@@ -3466,7 +3612,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>86</v>
       </c>
@@ -3498,7 +3644,9 @@
       <c r="K27" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L27" s="5"/>
+      <c r="L27" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M27" s="5" t="s">
         <v>140</v>
       </c>
@@ -3508,8 +3656,12 @@
       <c r="O27" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
+      <c r="P27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R27" s="5" t="s">
         <v>140</v>
       </c>
@@ -3544,7 +3696,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="174" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -3576,7 +3728,9 @@
       <c r="K28" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L28" s="5"/>
+      <c r="L28" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M28" s="5" t="s">
         <v>140</v>
       </c>
@@ -3626,7 +3780,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="116" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>92</v>
       </c>
@@ -3658,7 +3812,9 @@
       <c r="K29" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L29" s="5"/>
+      <c r="L29" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M29" s="5" t="s">
         <v>140</v>
       </c>
@@ -3706,7 +3862,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="174" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>95</v>
       </c>
@@ -3790,7 +3946,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>98</v>
       </c>
@@ -3822,7 +3978,9 @@
       <c r="K31" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L31" s="5"/>
+      <c r="L31" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M31" s="5" t="s">
         <v>140</v>
       </c>
@@ -3872,7 +4030,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>100</v>
       </c>
@@ -3904,7 +4062,9 @@
       <c r="K32" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L32" s="5"/>
+      <c r="L32" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M32" s="5" t="s">
         <v>140</v>
       </c>
@@ -3914,7 +4074,9 @@
       <c r="O32" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P32" s="5"/>
+      <c r="P32" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q32" s="5" t="s">
         <v>220</v>
       </c>
@@ -3952,7 +4114,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>103</v>
       </c>
@@ -3984,7 +4146,9 @@
       <c r="K33" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L33" s="5"/>
+      <c r="L33" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M33" s="5" t="s">
         <v>140</v>
       </c>
@@ -3994,8 +4158,12 @@
       <c r="O33" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
+      <c r="P33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R33" s="5" t="s">
         <v>140</v>
       </c>
@@ -4030,7 +4198,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>106</v>
       </c>
@@ -4062,7 +4230,9 @@
       <c r="K34" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L34" s="5"/>
+      <c r="L34" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M34" s="5" t="s">
         <v>140</v>
       </c>
@@ -4072,8 +4242,12 @@
       <c r="O34" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
+      <c r="P34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="R34" s="5" t="s">
         <v>140</v>
       </c>
@@ -4104,9 +4278,11 @@
       <c r="AA34" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB34" s="6"/>
-    </row>
-    <row r="35" spans="1:28" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="AB34" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>109</v>
       </c>
@@ -4138,7 +4314,9 @@
       <c r="K35" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L35" s="5"/>
+      <c r="L35" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="M35" s="5" t="s">
         <v>140</v>
       </c>
@@ -4148,7 +4326,9 @@
       <c r="O35" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="P35" s="5"/>
+      <c r="P35" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q35" s="5" t="s">
         <v>225</v>
       </c>
@@ -4164,7 +4344,9 @@
       <c r="U35" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V35" s="5"/>
+      <c r="V35" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W35" s="5" t="s">
         <v>140</v>
       </c>
@@ -4180,9 +4362,11 @@
       <c r="AA35" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="AB35" s="6"/>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB35" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K36" s="6"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
@@ -4202,7 +4386,7 @@
       <c r="AA36" s="6"/>
       <c r="AB36" s="6"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K37" s="6"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
@@ -4222,7 +4406,7 @@
       <c r="AA37" s="6"/>
       <c r="AB37" s="6"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K38" s="6"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
@@ -4242,7 +4426,7 @@
       <c r="AA38" s="6"/>
       <c r="AB38" s="6"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K39" s="6"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
@@ -4262,7 +4446,7 @@
       <c r="AA39" s="6"/>
       <c r="AB39" s="6"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K40" s="6"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
@@ -4282,7 +4466,7 @@
       <c r="AA40" s="6"/>
       <c r="AB40" s="6"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K41" s="6"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
@@ -4302,7 +4486,7 @@
       <c r="AA41" s="6"/>
       <c r="AB41" s="6"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K42" s="6"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
@@ -4322,7 +4506,7 @@
       <c r="AA42" s="6"/>
       <c r="AB42" s="6"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K43" s="6"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
@@ -4342,7 +4526,7 @@
       <c r="AA43" s="6"/>
       <c r="AB43" s="6"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K44" s="6"/>
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
@@ -4362,7 +4546,7 @@
       <c r="AA44" s="6"/>
       <c r="AB44" s="6"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K45" s="6"/>
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
@@ -4382,7 +4566,7 @@
       <c r="AA45" s="6"/>
       <c r="AB45" s="6"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K46" s="6"/>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
@@ -4402,7 +4586,7 @@
       <c r="AA46" s="6"/>
       <c r="AB46" s="6"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K47" s="6"/>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
@@ -4422,7 +4606,7 @@
       <c r="AA47" s="6"/>
       <c r="AB47" s="6"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K48" s="6"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
@@ -4442,7 +4626,7 @@
       <c r="AA48" s="6"/>
       <c r="AB48" s="6"/>
     </row>
-    <row r="49" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="49" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K49" s="6"/>
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
@@ -4462,7 +4646,7 @@
       <c r="AA49" s="6"/>
       <c r="AB49" s="6"/>
     </row>
-    <row r="50" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="50" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K50" s="6"/>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
@@ -4482,7 +4666,7 @@
       <c r="AA50" s="6"/>
       <c r="AB50" s="6"/>
     </row>
-    <row r="51" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="51" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K51" s="6"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
@@ -4502,7 +4686,7 @@
       <c r="AA51" s="6"/>
       <c r="AB51" s="6"/>
     </row>
-    <row r="52" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="52" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K52" s="6"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
@@ -4522,7 +4706,7 @@
       <c r="AA52" s="6"/>
       <c r="AB52" s="6"/>
     </row>
-    <row r="53" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="53" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K53" s="6"/>
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
@@ -4542,7 +4726,7 @@
       <c r="AA53" s="6"/>
       <c r="AB53" s="6"/>
     </row>
-    <row r="54" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="54" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K54" s="6"/>
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
@@ -4562,7 +4746,7 @@
       <c r="AA54" s="6"/>
       <c r="AB54" s="6"/>
     </row>
-    <row r="55" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="55" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K55" s="6"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
@@ -4582,7 +4766,7 @@
       <c r="AA55" s="6"/>
       <c r="AB55" s="6"/>
     </row>
-    <row r="56" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="56" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K56" s="6"/>
       <c r="L56" s="5"/>
       <c r="M56" s="5"/>
@@ -4602,7 +4786,7 @@
       <c r="AA56" s="6"/>
       <c r="AB56" s="6"/>
     </row>
-    <row r="57" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="57" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K57" s="6"/>
       <c r="L57" s="5"/>
       <c r="M57" s="5"/>
@@ -4622,7 +4806,7 @@
       <c r="AA57" s="6"/>
       <c r="AB57" s="6"/>
     </row>
-    <row r="58" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="58" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K58" s="6"/>
       <c r="L58" s="5"/>
       <c r="M58" s="5"/>
@@ -4642,7 +4826,7 @@
       <c r="AA58" s="6"/>
       <c r="AB58" s="6"/>
     </row>
-    <row r="59" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="59" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K59" s="6"/>
       <c r="L59" s="5"/>
       <c r="M59" s="5"/>
@@ -4662,7 +4846,7 @@
       <c r="AA59" s="6"/>
       <c r="AB59" s="6"/>
     </row>
-    <row r="60" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="60" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K60" s="6"/>
       <c r="L60" s="5"/>
       <c r="M60" s="5"/>
@@ -4682,7 +4866,7 @@
       <c r="AA60" s="6"/>
       <c r="AB60" s="6"/>
     </row>
-    <row r="61" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="61" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K61" s="6"/>
       <c r="L61" s="5"/>
       <c r="M61" s="5"/>
@@ -4702,7 +4886,7 @@
       <c r="AA61" s="6"/>
       <c r="AB61" s="6"/>
     </row>
-    <row r="62" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="62" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K62" s="6"/>
       <c r="L62" s="5"/>
       <c r="M62" s="5"/>
@@ -4722,7 +4906,7 @@
       <c r="AA62" s="6"/>
       <c r="AB62" s="6"/>
     </row>
-    <row r="63" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="63" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K63" s="6"/>
       <c r="L63" s="5"/>
       <c r="M63" s="5"/>
@@ -4742,7 +4926,7 @@
       <c r="AA63" s="6"/>
       <c r="AB63" s="6"/>
     </row>
-    <row r="64" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="64" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K64" s="6"/>
       <c r="L64" s="5"/>
       <c r="M64" s="5"/>
@@ -4762,7 +4946,7 @@
       <c r="AA64" s="6"/>
       <c r="AB64" s="6"/>
     </row>
-    <row r="65" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="65" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K65" s="6"/>
       <c r="L65" s="5"/>
       <c r="M65" s="5"/>
@@ -4782,7 +4966,7 @@
       <c r="AA65" s="6"/>
       <c r="AB65" s="6"/>
     </row>
-    <row r="66" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="66" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K66" s="6"/>
       <c r="L66" s="5"/>
       <c r="M66" s="5"/>
@@ -4802,7 +4986,7 @@
       <c r="AA66" s="6"/>
       <c r="AB66" s="6"/>
     </row>
-    <row r="67" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="67" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K67" s="6"/>
       <c r="L67" s="5"/>
       <c r="M67" s="5"/>
@@ -4822,7 +5006,7 @@
       <c r="AA67" s="6"/>
       <c r="AB67" s="6"/>
     </row>
-    <row r="68" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="68" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K68" s="6"/>
       <c r="L68" s="5"/>
       <c r="M68" s="5"/>
@@ -4842,7 +5026,7 @@
       <c r="AA68" s="6"/>
       <c r="AB68" s="6"/>
     </row>
-    <row r="69" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="69" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K69" s="6"/>
       <c r="L69" s="5"/>
       <c r="M69" s="5"/>
@@ -4862,7 +5046,7 @@
       <c r="AA69" s="6"/>
       <c r="AB69" s="6"/>
     </row>
-    <row r="70" spans="11:28" x14ac:dyDescent="0.35">
+    <row r="70" spans="11:28" x14ac:dyDescent="0.3">
       <c r="K70" s="6"/>
       <c r="L70" s="5"/>
       <c r="M70" s="5"/>

</xml_diff>

<commit_message>
update preparation.md, create old-folder. Add columns with filters in tables for annotation
</commit_message>
<xml_diff>
--- a/titlePilotStudy/data/ITL.xlsx
+++ b/titlePilotStudy/data/ITL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HU-BOX\Seafile\COST\dataTitleStudy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HU-GIT\COST\WG1\titlePilotStudy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="173">
   <si>
     <t>ITBI0087</t>
   </si>
@@ -505,75 +505,6 @@
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>senilità</t>
-  </si>
-  <si>
-    <t>indef</t>
-  </si>
-  <si>
-    <t>vita</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>pinocchio</t>
-  </si>
-  <si>
-    <t>sposi</t>
-  </si>
-  <si>
-    <t>croci</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>avventure</t>
-  </si>
-  <si>
-    <t>def</t>
-  </si>
-  <si>
-    <t>piccolo mondo</t>
-  </si>
-  <si>
-    <t>processi verbali</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>occhi</t>
-  </si>
-  <si>
-    <t>more</t>
-  </si>
-  <si>
-    <t>fede, bellezza</t>
-  </si>
-  <si>
-    <t>word</t>
-  </si>
-  <si>
-    <t>daniele cortis</t>
-  </si>
-  <si>
-    <t>cuore</t>
-  </si>
-  <si>
-    <t>zeno</t>
-  </si>
-  <si>
-    <t>coscienza</t>
   </si>
   <si>
     <r>
@@ -606,9 +537,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> romanzo</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Senso. </t>
     </r>
@@ -622,9 +550,6 @@
       </rPr>
       <t>Nuove storielle vane</t>
     </r>
-  </si>
-  <si>
-    <t>senso</t>
   </si>
   <si>
     <r>
@@ -674,9 +599,6 @@
     </r>
   </si>
   <si>
-    <t>romanzo</t>
-  </si>
-  <si>
     <r>
       <t>Cantoni il volontario</t>
     </r>
@@ -692,15 +614,6 @@
     </r>
   </si>
   <si>
-    <t>volontario</t>
-  </si>
-  <si>
-    <t>cantoni</t>
-  </si>
-  <si>
-    <t>carso</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Cent'anni/  </t>
     </r>
@@ -714,9 +627,6 @@
       </rPr>
       <t>Cento anni: Romanzo ciclico???</t>
     </r>
-  </si>
-  <si>
-    <t>anni</t>
   </si>
   <si>
     <r>
@@ -735,18 +645,6 @@
     </r>
   </si>
   <si>
-    <t>clelia</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>governo</t>
-  </si>
-  <si>
-    <t>mixed</t>
-  </si>
-  <si>
     <r>
       <t>Dio ne scampi dagli Orsenigo</t>
     </r>
@@ -762,12 +660,6 @@
     </r>
   </si>
   <si>
-    <t>orsenigo</t>
-  </si>
-  <si>
-    <t>dio</t>
-  </si>
-  <si>
     <r>
       <t>Fosca</t>
     </r>
@@ -783,18 +675,6 @@
     </r>
   </si>
   <si>
-    <t>fosca</t>
-  </si>
-  <si>
-    <t>Ponte Nuovo</t>
-  </si>
-  <si>
-    <t>Pasquale Paoli</t>
-  </si>
-  <si>
-    <t>rotta</t>
-  </si>
-  <si>
     <r>
       <t>Pasquale Paoli, ossia La rotta di Ponte Nuovo</t>
     </r>
@@ -810,12 +690,6 @@
     </r>
   </si>
   <si>
-    <t>Palazzo Carignano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moribondi </t>
-  </si>
-  <si>
     <r>
       <t>Il marito di Elena</t>
     </r>
@@ -846,24 +720,6 @@
     </r>
   </si>
   <si>
-    <t>viceré</t>
-  </si>
-  <si>
-    <t>elena, marito</t>
-  </si>
-  <si>
-    <t>marito</t>
-  </si>
-  <si>
-    <t>freccia</t>
-  </si>
-  <si>
-    <t>piacere</t>
-  </si>
-  <si>
-    <t>fianco</t>
-  </si>
-  <si>
     <r>
       <t>La freccia nel fianco</t>
     </r>
@@ -894,9 +750,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">mano </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">La scapigliatura e il 6 febbrajo. </t>
     </r>
@@ -912,15 +765,6 @@
     </r>
   </si>
   <si>
-    <t>scapigliatura</t>
-  </si>
-  <si>
-    <t>6 febbrajo, dramma, famiglia</t>
-  </si>
-  <si>
-    <t>un dramma in famiglia, romanzo contemporano di cletto arrighi</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Le confessioni d'un Italiano/ </t>
     </r>
@@ -936,15 +780,6 @@
     </r>
   </si>
   <si>
-    <t>italiano, ottuagenario</t>
-  </si>
-  <si>
-    <t>confesioni</t>
-  </si>
-  <si>
-    <t>confessioni</t>
-  </si>
-  <si>
     <r>
       <t>Lorenzo Benoni, ovvero scene della vita di un italiano</t>
     </r>
@@ -960,15 +795,6 @@
     </r>
   </si>
   <si>
-    <t>scene</t>
-  </si>
-  <si>
-    <t>italiano</t>
-  </si>
-  <si>
-    <t>Lorenzo Benoni</t>
-  </si>
-  <si>
     <r>
       <t>Il sorbetto della regina</t>
     </r>
@@ -984,18 +810,6 @@
     </r>
   </si>
   <si>
-    <t>regina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sorbetto </t>
-  </si>
-  <si>
-    <t>giuda</t>
-  </si>
-  <si>
-    <t>memorie</t>
-  </si>
-  <si>
     <r>
       <t>Profumo</t>
     </r>
@@ -1011,35 +825,47 @@
     </r>
   </si>
   <si>
-    <t>profumo</t>
-  </si>
-  <si>
-    <t>tigre</t>
-  </si>
-  <si>
-    <t>peccatrice</t>
-  </si>
-  <si>
-    <t>storia</t>
-  </si>
-  <si>
-    <t>libro</t>
-  </si>
-  <si>
-    <t>storielle</t>
-  </si>
-  <si>
-    <t>racconto</t>
-  </si>
-  <si>
-    <t>scene, pagine</t>
+    <t>index</t>
+  </si>
+  <si>
+    <t>placeRole</t>
+  </si>
+  <si>
+    <t>placeSyntax</t>
+  </si>
+  <si>
+    <t>personRole</t>
+  </si>
+  <si>
+    <t>personSyntax</t>
+  </si>
+  <si>
+    <t>personIIRole</t>
+  </si>
+  <si>
+    <t>personIISyntax</t>
+  </si>
+  <si>
+    <t>otherEntityRole</t>
+  </si>
+  <si>
+    <t>otherEntitySyntax</t>
+  </si>
+  <si>
+    <t>otherEntityIIRole</t>
+  </si>
+  <si>
+    <t>otherEntityIISyntax</t>
+  </si>
+  <si>
+    <t>titleFocus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1089,6 +915,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1111,7 +944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1131,10 +964,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1418,17 +1255,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB70"/>
+  <dimension ref="A1:AN70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O1" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="AB1" sqref="AB1"/>
+      <selection pane="bottomLeft" activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="30" max="30" width="8.88671875" style="9"/>
+    <col min="31" max="31" width="12.6640625" style="9" customWidth="1"/>
+    <col min="32" max="32" width="8.21875" style="9" customWidth="1"/>
+    <col min="33" max="33" width="7.88671875" style="9" customWidth="1"/>
+    <col min="34" max="34" width="10.21875" style="9" customWidth="1"/>
+    <col min="35" max="35" width="11.6640625" style="9" customWidth="1"/>
+    <col min="36" max="36" width="9" style="9" customWidth="1"/>
+    <col min="37" max="40" width="10.88671875" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -1513,8 +1360,44 @@
       <c r="AB1" s="4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AC1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1574,10 +1457,10 @@
         <v>140</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>140</v>
@@ -1585,20 +1468,56 @@
       <c r="X2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y2" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1658,31 +1577,67 @@
         <v>140</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y3" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN3" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1724,13 +1679,13 @@
         <v>140</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>140</v>
@@ -1739,34 +1694,70 @@
         <v>140</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y4" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN4" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1796,13 +1787,13 @@
         <v>21</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>140</v>
@@ -1837,20 +1828,56 @@
       <c r="X5" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y5" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB5" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI5" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ5" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK5" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL5" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM5" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN5" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1910,31 +1937,67 @@
         <v>140</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="W6" s="5" t="s">
         <v>140</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA6" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI6" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ6" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK6" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL6" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM6" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN6" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1952,7 +2015,7 @@
         <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>28</v>
@@ -1976,47 +2039,85 @@
         <v>140</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="U7" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="V7" s="5"/>
+      <c r="V7" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="W7" s="5" t="s">
         <v>140</v>
       </c>
       <c r="X7" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y7" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN7" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -2076,31 +2177,67 @@
         <v>140</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="W8" s="5" t="s">
         <v>140</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y8" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z8" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA8" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB8" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI8" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ8" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK8" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL8" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM8" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN8" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -2160,31 +2297,67 @@
         <v>140</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z9" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA9" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI9" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK9" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL9" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM9" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN9" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -2213,7 +2386,7 @@
       <c r="J10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="5" t="s">
         <v>140</v>
       </c>
       <c r="L10" s="5" t="s">
@@ -2244,10 +2417,10 @@
         <v>140</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="W10" s="5" t="s">
         <v>140</v>
@@ -2255,20 +2428,56 @@
       <c r="X10" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y10" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z10" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AA10" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB10" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN10" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -2286,7 +2495,7 @@
         <v>41</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>20</v>
@@ -2297,7 +2506,7 @@
       <c r="J11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="5" t="s">
         <v>140</v>
       </c>
       <c r="L11" s="5" t="s">
@@ -2310,13 +2519,13 @@
         <v>140</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="R11" s="5" t="s">
         <v>140</v>
@@ -2325,7 +2534,7 @@
         <v>140</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U11" s="5" t="s">
         <v>140</v>
@@ -2339,20 +2548,56 @@
       <c r="X11" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y11" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z11" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA11" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB11" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI11" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ11" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK11" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL11" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM11" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN11" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -2370,7 +2615,7 @@
         <v>23</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>43</v>
@@ -2381,7 +2626,7 @@
       <c r="J12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="5" t="s">
         <v>140</v>
       </c>
       <c r="L12" s="5" t="s">
@@ -2394,13 +2639,13 @@
         <v>140</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="R12" s="5" t="s">
         <v>140</v>
@@ -2409,7 +2654,7 @@
         <v>140</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U12" s="5" t="s">
         <v>140</v>
@@ -2423,20 +2668,56 @@
       <c r="X12" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y12" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z12" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA12" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB12" s="6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Y12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI12" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ12" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK12" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL12" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM12" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN12" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -2454,7 +2735,7 @@
         <v>45</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>5</v>
@@ -2484,43 +2765,79 @@
         <v>140</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="S13" s="5" t="s">
         <v>140</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="W13" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X13" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y13" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z13" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA13" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB13" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Y13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI13" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ13" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK13" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL13" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM13" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN13" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -2538,7 +2855,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>47</v>
@@ -2580,10 +2897,10 @@
         <v>140</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="W14" s="5" t="s">
         <v>140</v>
@@ -2591,20 +2908,56 @@
       <c r="X14" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y14" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z14" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA14" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB14" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI14" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ14" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK14" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL14" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM14" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN14" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
@@ -2646,22 +2999,22 @@
         <v>140</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P15" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U15" s="5" t="s">
         <v>140</v>
@@ -2675,20 +3028,56 @@
       <c r="X15" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y15" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z15" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA15" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB15" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="Y15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI15" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ15" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK15" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL15" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM15" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN15" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -2706,7 +3095,7 @@
         <v>53</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>54</v>
@@ -2730,22 +3119,22 @@
         <v>140</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="S16" s="5" t="s">
         <v>140</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U16" s="5" t="s">
         <v>140</v>
@@ -2759,20 +3148,56 @@
       <c r="X16" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y16" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z16" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA16" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB16" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Y16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI16" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ16" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK16" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL16" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM16" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN16" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>55</v>
       </c>
@@ -2790,7 +3215,7 @@
         <v>56</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>57</v>
@@ -2832,31 +3257,67 @@
         <v>140</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V17" s="5" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="W17" s="5" t="s">
         <v>140</v>
       </c>
       <c r="X17" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y17" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z17" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA17" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB17" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" ht="345.6" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="Y17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI17" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ17" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK17" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL17" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM17" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN17" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
@@ -2874,7 +3335,7 @@
         <v>53</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>54</v>
@@ -2898,13 +3359,13 @@
         <v>140</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="R18" s="5" t="s">
         <v>140</v>
@@ -2913,34 +3374,70 @@
         <v>140</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="V18" s="5" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="W18" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y18" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z18" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA18" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB18" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="Y18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI18" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ18" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK18" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL18" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM18" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN18" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -2958,7 +3455,7 @@
         <v>60</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>61</v>
@@ -2982,49 +3479,85 @@
         <v>140</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="R19" s="5" t="s">
         <v>140</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V19" s="5" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="W19" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X19" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y19" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z19" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA19" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB19" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Y19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI19" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ19" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK19" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL19" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM19" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN19" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -3042,7 +3575,7 @@
         <v>63</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>64</v>
@@ -3066,13 +3599,13 @@
         <v>140</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>187</v>
+        <v>140</v>
       </c>
       <c r="R20" s="5" t="s">
         <v>140</v>
@@ -3081,7 +3614,7 @@
         <v>140</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="U20" s="5" t="s">
         <v>140</v>
@@ -3095,20 +3628,56 @@
       <c r="X20" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y20" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z20" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA20" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB20" s="6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="Y20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI20" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ20" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK20" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL20" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM20" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN20" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>65</v>
       </c>
@@ -3126,7 +3695,7 @@
         <v>66</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>67</v>
@@ -3138,25 +3707,25 @@
         <v>21</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>188</v>
+        <v>140</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="N21" s="5" t="s">
         <v>140</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="R21" s="5" t="s">
         <v>140</v>
@@ -3165,34 +3734,70 @@
         <v>140</v>
       </c>
       <c r="T21" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U21" s="5" t="s">
         <v>140</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="W21" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y21" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z21" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA21" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB21" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" ht="72" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="Y21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI21" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ21" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK21" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL21" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM21" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN21" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
@@ -3222,34 +3827,34 @@
         <v>21</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="M22" s="5" t="s">
         <v>140</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>193</v>
+        <v>140</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="T22" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U22" s="5" t="s">
         <v>140</v>
@@ -3263,20 +3868,56 @@
       <c r="X22" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y22" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z22" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA22" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB22" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI22" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ22" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK22" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL22" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM22" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN22" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>72</v>
       </c>
@@ -3294,7 +3935,7 @@
         <v>73</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>74</v>
@@ -3318,22 +3959,22 @@
         <v>140</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="R23" s="5" t="s">
         <v>140</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U23" s="5" t="s">
         <v>140</v>
@@ -3347,20 +3988,56 @@
       <c r="X23" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y23" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z23" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA23" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB23" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" ht="72" x14ac:dyDescent="0.3">
+      <c r="Y23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI23" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ23" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK23" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL23" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM23" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN23" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>75</v>
       </c>
@@ -3378,7 +4055,7 @@
         <v>76</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>77</v>
@@ -3402,22 +4079,22 @@
         <v>140</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>198</v>
+        <v>140</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="U24" s="5" t="s">
         <v>140</v>
@@ -3431,20 +4108,56 @@
       <c r="X24" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y24" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z24" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA24" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB24" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI24" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ24" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK24" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL24" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM24" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN24" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>78</v>
       </c>
@@ -3504,31 +4217,67 @@
         <v>140</v>
       </c>
       <c r="U25" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V25" s="5" t="s">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="W25" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X25" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y25" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z25" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA25" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB25" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN25" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>83</v>
       </c>
@@ -3546,7 +4295,7 @@
         <v>84</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>85</v>
@@ -3558,16 +4307,16 @@
         <v>21</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="O26" s="5" t="s">
         <v>140</v>
@@ -3588,31 +4337,67 @@
         <v>140</v>
       </c>
       <c r="U26" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>199</v>
+        <v>140</v>
       </c>
       <c r="W26" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X26" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y26" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z26" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA26" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB26" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Y26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI26" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ26" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK26" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL26" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM26" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN26" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>86</v>
       </c>
@@ -3630,7 +4415,7 @@
         <v>87</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>203</v>
+        <v>155</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>88</v>
@@ -3672,31 +4457,67 @@
         <v>140</v>
       </c>
       <c r="U27" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="W27" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X27" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y27" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z27" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA27" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB27" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" ht="172.8" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="Y27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI27" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ27" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK27" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL27" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM27" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN27" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -3714,7 +4535,7 @@
         <v>90</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>205</v>
+        <v>156</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>91</v>
@@ -3738,49 +4559,85 @@
         <v>140</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>206</v>
+        <v>140</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>206</v>
+        <v>140</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="T28" s="5" t="s">
         <v>140</v>
       </c>
       <c r="U28" s="5" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="V28" s="5" t="s">
-        <v>207</v>
+        <v>140</v>
       </c>
       <c r="W28" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="X28" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y28" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z28" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA28" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB28" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="Y28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI28" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ28" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK28" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL28" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM28" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN28" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>92</v>
       </c>
@@ -3798,7 +4655,7 @@
         <v>93</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>209</v>
+        <v>157</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>94</v>
@@ -3822,47 +4679,85 @@
         <v>140</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="P29" s="5"/>
+        <v>140</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="Q29" s="5" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="R29" s="5" t="s">
         <v>140</v>
       </c>
       <c r="S29" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U29" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V29" s="5" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="W29" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X29" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y29" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z29" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA29" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB29" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="Y29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI29" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ29" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK29" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL29" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM29" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN29" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>95</v>
       </c>
@@ -3880,7 +4775,7 @@
         <v>96</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>97</v>
@@ -3892,25 +4787,25 @@
         <v>21</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="N30" s="5" t="s">
         <v>140</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P30" s="5" t="s">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="Q30" s="5" t="s">
-        <v>216</v>
+        <v>140</v>
       </c>
       <c r="R30" s="5" t="s">
         <v>140</v>
@@ -3919,34 +4814,70 @@
         <v>140</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U30" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V30" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="W30" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X30" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y30" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z30" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AA30" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB30" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" ht="72" x14ac:dyDescent="0.3">
+      <c r="Y30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI30" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ30" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK30" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL30" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM30" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN30" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>98</v>
       </c>
@@ -3964,7 +4895,7 @@
         <v>99</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>71</v>
@@ -3988,49 +4919,85 @@
         <v>140</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P31" s="5" t="s">
-        <v>218</v>
+        <v>140</v>
       </c>
       <c r="Q31" s="5" t="s">
-        <v>218</v>
+        <v>140</v>
       </c>
       <c r="R31" s="5" t="s">
         <v>140</v>
       </c>
       <c r="S31" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="U31" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V31" s="5" t="s">
-        <v>219</v>
+        <v>140</v>
       </c>
       <c r="W31" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X31" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y31" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z31" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA31" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB31" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" ht="72" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="Y31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI31" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ31" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK31" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL31" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM31" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN31" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>100</v>
       </c>
@@ -4072,49 +5039,85 @@
         <v>140</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P32" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="S32" s="5" t="s">
         <v>140</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U32" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V32" s="5" t="s">
-        <v>221</v>
+        <v>140</v>
       </c>
       <c r="W32" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="X32" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y32" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z32" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA32" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB32" s="6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Y32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI32" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ32" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK32" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL32" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM32" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN32" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>103</v>
       </c>
@@ -4132,7 +5135,7 @@
         <v>104</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>222</v>
+        <v>160</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>105</v>
@@ -4174,10 +5177,10 @@
         <v>140</v>
       </c>
       <c r="U33" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V33" s="5" t="s">
-        <v>223</v>
+        <v>140</v>
       </c>
       <c r="W33" s="5" t="s">
         <v>140</v>
@@ -4185,20 +5188,56 @@
       <c r="X33" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y33" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z33" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA33" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB33" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Y33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI33" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ33" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK33" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL33" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM33" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN33" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>106</v>
       </c>
@@ -4258,31 +5297,67 @@
         <v>140</v>
       </c>
       <c r="U34" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V34" s="5" t="s">
-        <v>224</v>
+        <v>140</v>
       </c>
       <c r="W34" s="5" t="s">
         <v>140</v>
       </c>
       <c r="X34" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y34" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z34" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA34" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB34" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI34" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ34" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK34" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL34" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM34" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN34" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>109</v>
       </c>
@@ -4324,22 +5399,22 @@
         <v>140</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="P35" s="5" t="s">
         <v>140</v>
       </c>
       <c r="Q35" s="5" t="s">
-        <v>225</v>
+        <v>140</v>
       </c>
       <c r="R35" s="5" t="s">
         <v>140</v>
       </c>
       <c r="S35" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="U35" s="5" t="s">
         <v>140</v>
@@ -4353,20 +5428,56 @@
       <c r="X35" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="Y35" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z35" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA35" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB35" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="Y35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI35" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ35" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK35" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL35" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM35" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN35" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K36" s="6"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
@@ -4386,7 +5497,7 @@
       <c r="AA36" s="6"/>
       <c r="AB36" s="6"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K37" s="6"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
@@ -4406,7 +5517,7 @@
       <c r="AA37" s="6"/>
       <c r="AB37" s="6"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K38" s="6"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
@@ -4426,7 +5537,7 @@
       <c r="AA38" s="6"/>
       <c r="AB38" s="6"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K39" s="6"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
@@ -4446,7 +5557,7 @@
       <c r="AA39" s="6"/>
       <c r="AB39" s="6"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K40" s="6"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
@@ -4466,7 +5577,7 @@
       <c r="AA40" s="6"/>
       <c r="AB40" s="6"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K41" s="6"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
@@ -4486,7 +5597,7 @@
       <c r="AA41" s="6"/>
       <c r="AB41" s="6"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K42" s="6"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
@@ -4506,7 +5617,7 @@
       <c r="AA42" s="6"/>
       <c r="AB42" s="6"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K43" s="6"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
@@ -4526,7 +5637,7 @@
       <c r="AA43" s="6"/>
       <c r="AB43" s="6"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K44" s="6"/>
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
@@ -4546,7 +5657,7 @@
       <c r="AA44" s="6"/>
       <c r="AB44" s="6"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K45" s="6"/>
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
@@ -4566,7 +5677,7 @@
       <c r="AA45" s="6"/>
       <c r="AB45" s="6"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K46" s="6"/>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
@@ -4586,7 +5697,7 @@
       <c r="AA46" s="6"/>
       <c r="AB46" s="6"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K47" s="6"/>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
@@ -4606,7 +5717,7 @@
       <c r="AA47" s="6"/>
       <c r="AB47" s="6"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
       <c r="K48" s="6"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
@@ -5067,21 +6178,27 @@
       <c r="AB70" s="6"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K35 O1:O70 AA1:AA70 R1:R70 M1:M70 X1:Y70">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X36:Y70 X1:Y1 AB2:AN35 L2:L35 N2:N35 P2:Q35 S2:Z35 O1:O70 AA1:AA70 R1:R70 M1:M70 K1:K35">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1 T36:T70">
       <formula1>"m,f,d,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1 U36:U70">
       <formula1>"one,more,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1 Z36:Z70">
       <formula1>"interpunc,word,mixed,none"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1:W70 N1:N70 S1:S70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S36:S70 W36:W70 S1 N1 W1 N36:N70">
       <formula1>"def,indef,no"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI36:AI1048576 AK36:AK1048576 AM36:AM1048576 AE36:AE1048576 AM1 AK1 AI1 AG1 AE1 AG36:AG1048576">
+      <formula1>"head,apposition,pregen,postgen,prepmod,adjective,no"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH36:AH1048576 AJ36:AJ1048576 AL36:AL1048576 AD36:AD1048576 AL1 AJ1 AH1 AF1 AD1 AF36:AF1048576">
+      <formula1>"existence,possessor,possessum,patient,location,agens,attribute,no"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>